<commit_message>
Initial ProductBacklog and SprintBacklog
</commit_message>
<xml_diff>
--- a/Scrum_Log_Book.xlsx
+++ b/Scrum_Log_Book.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Takuya\Documents\Coventry\Rapid Application Development\Assignment2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="5175"/>
   </bookViews>
@@ -19,7 +14,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>Kayen</t>
   </si>
@@ -76,6 +71,66 @@
   </si>
   <si>
     <t>Successfully getting and displaying JSON file (taxi locations) from http://datamall2.mytransport.sg/.</t>
+  </si>
+  <si>
+    <t>Contribute to repository via Git</t>
+  </si>
+  <si>
+    <t>Learn Google App Engine code</t>
+  </si>
+  <si>
+    <t>ProuctBacklog</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Current Location</t>
+  </si>
+  <si>
+    <t>Pb_id</t>
+  </si>
+  <si>
+    <t>I want to see my current location on google map.</t>
+  </si>
+  <si>
+    <t>Taxi Location</t>
+  </si>
+  <si>
+    <t>I want to see nearby available taxis on google map</t>
+  </si>
+  <si>
+    <t>Delivery Date</t>
+  </si>
+  <si>
+    <t>Sb_id</t>
+  </si>
+  <si>
+    <t>SprintBacklog</t>
+  </si>
+  <si>
+    <t>TaxiAvailability API header</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Need to get API key and other header information</t>
+  </si>
+  <si>
+    <t>JINJA2</t>
+  </si>
+  <si>
+    <t>Use JINJA2 template for MVC framework</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Implement current location in JavaScript in accordance with Google Map API</t>
   </si>
 </sst>
 </file>
@@ -410,7 +465,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>352425</xdr:rowOff>
+      <xdr:rowOff>533400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="936282" cy="405432"/>
     <xdr:sp macro="" textlink="">
@@ -420,7 +475,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="7991475"/>
+          <a:off x="0" y="13325475"/>
           <a:ext cx="936282" cy="405432"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -507,7 +562,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -542,7 +597,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -719,7 +774,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -729,9 +784,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,11 +861,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="G6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="3:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
@@ -1133,26 +1192,193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Spring backlog updated on 22nd Sep
</commit_message>
<xml_diff>
--- a/Scrum_Log_Book.xlsx
+++ b/Scrum_Log_Book.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
   <si>
     <t>Thu</t>
   </si>
@@ -372,9 +372,6 @@
     <t>To demonstrate prototype UI design (format) on 22nd September</t>
   </si>
   <si>
-    <t>To demonstrate prototype UI design (Colour) on 22nd September</t>
-  </si>
-  <si>
     <t>To demonstrate progress of Map Unification on 22nd September</t>
   </si>
   <si>
@@ -382,6 +379,33 @@
   </si>
   <si>
     <t>Kayen</t>
+  </si>
+  <si>
+    <t>Scrum meeting for progress reporting and to agree with product backlog and sprint backlog for sprint2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scrum meeting for progress reporting and show latest UI design. Due to technical difficulty, postponed UI design demo date. Agreed with finishing up all the tasks by end of this week. </t>
+  </si>
+  <si>
+    <t>To demonstrate prototype UI design (colour) on 22nd September</t>
+  </si>
+  <si>
+    <t>Scrum meeting for progress reporting and show latest UI design. UI design was demonstrated but not integrated. Agreed with finishing up all the tasks by end of this week. Sprint backlog updated.</t>
+  </si>
+  <si>
+    <t>To demonstrate Distance Computation (without unit conversion) by noon on 25th September</t>
+  </si>
+  <si>
+    <t>To demonstrate integrated UI design (format) by end of 24th September</t>
+  </si>
+  <si>
+    <t>To demonstrate integrated UI design (colour) by end of 24th September</t>
+  </si>
+  <si>
+    <t>To integrate code and UI design then upload relevant files to Github by end of 25th September</t>
+  </si>
+  <si>
+    <t>--</t>
   </si>
 </sst>
 </file>
@@ -430,7 +454,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +464,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -570,6 +600,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1279,8 +1317,8 @@
   <dimension ref="C2:H37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,16 +1651,16 @@
         <v>2</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>74</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1634,7 +1672,9 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="3:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1646,7 +1686,9 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="3:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1656,10 +1698,18 @@
       <c r="D24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="25" spans="3:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
@@ -1777,7 +1827,7 @@
   <dimension ref="B6:E12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1895,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F63"/>
+  <dimension ref="B2:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,27 +2131,37 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="B12" s="12">
+        <v>1.2</v>
+      </c>
+      <c r="C12" s="10">
+        <v>10</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="11">
+        <v>42625</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <v>1.2</v>
       </c>
       <c r="C13" s="10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E13" s="11">
-        <v>42625</v>
+        <v>42627</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -2109,33 +2169,33 @@
         <v>1.2</v>
       </c>
       <c r="C14" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E14" s="11">
-        <v>42627</v>
+        <v>42628</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
         <v>1.2</v>
       </c>
       <c r="C15" s="10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="11">
         <v>42628</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2143,64 +2203,68 @@
         <v>1.2</v>
       </c>
       <c r="C16" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="E16" s="11">
-        <v>42628</v>
+        <v>42629</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="12">
         <v>1.2</v>
       </c>
       <c r="C17" s="10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E17" s="11">
         <v>42629</v>
       </c>
       <c r="F17" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="12">
+        <v>2.1</v>
+      </c>
+      <c r="C19" s="10">
+        <v>15</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="21">
+        <v>42635</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
-        <v>1.2</v>
-      </c>
-      <c r="C18" s="10">
-        <v>15</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="11">
-        <v>42629</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="12">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C20" s="10">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E20" s="21">
         <v>42635</v>
@@ -2211,10 +2275,10 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C21" s="10">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>77</v>
@@ -2223,15 +2287,15 @@
         <v>42635</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="12">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="C22" s="10">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>78</v>
@@ -2240,43 +2304,94 @@
         <v>42635</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
+        <v>2.1</v>
+      </c>
+      <c r="C23" s="10">
+        <v>19</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="21">
+        <v>42637</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C24" s="10">
+        <v>20</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="21">
+        <v>42637</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
         <v>2.4</v>
       </c>
-      <c r="C23" s="10">
-        <v>18</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C25" s="10">
+        <v>21</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="21">
+        <v>42638</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="21">
-        <v>42635</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>80</v>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="10">
+        <v>22</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="21">
+        <v>42638</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>